<commit_message>
added example output in the text folder
</commit_message>
<xml_diff>
--- a/2023_analysis/data/chilkat_sockeye_template.xlsx
+++ b/2023_analysis/data/chilkat_sockeye_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Chilkat_sockeye_state_space_model\2023_analysis\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3229CC21-BA14-493C-A00A-D0A502B62AAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A129462D-5D61-4CBB-9677-875BB3C86F8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -57,7 +57,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">Make sure the spreadsheet Chilkat Lake DIDSON-daily counts 2008-2020 20 April 21 is updated to reflect any DIDSON expansion. This will carry over to the 'Chikat sockeye weighted age comp.' spreadsheet and the brood table spreadsheet, 'age' sheet. 
+          <t xml:space="preserve">Make sure the spreadsheet Chilkat Lake DIDSON-daily counts 2008-2022 is updated to reflect any DIDSON expansion. This will carry over to the 'Chikat sockeye weighted age comp.' spreadsheet and the brood table spreadsheet, 'age' sheet. 
 </t>
         </r>
       </text>
@@ -70,7 +70,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">SEM: 3/20/2023 </t>
         </r>
@@ -81,7 +81,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">verify how these were calculated
+          <t xml:space="preserve">verify 0.05 if not expanded; 0.1 if expanded early OR late; 0.2 if expanded for both early and late
 </t>
         </r>
       </text>
@@ -94,7 +94,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">SEM; 3-17-2023: </t>
         </r>
@@ -113,7 +113,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve"> </t>
         </r>
@@ -122,7 +122,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 </t>
@@ -148,7 +148,26 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">From the brood table spreadsheet, 'age' tab.
+          <t xml:space="preserve">From the brood table spreadsheet, 'age' tab. Look at table </t>
+        </r>
+        <r>
+          <rPr>
+            <i/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Total Run (effective sample size); </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">make sure these are whole numbers!
 </t>
         </r>
       </text>
@@ -206,7 +225,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="22" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -345,19 +364,6 @@
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
       <family val="2"/>
     </font>
     <font>
@@ -367,8 +373,15 @@
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
+    <font>
+      <i/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="34">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -546,12 +559,6 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -715,11 +722,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1078,7 +1083,7 @@
   <dimension ref="A1:U48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="L22" sqref="L22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1153,13 +1158,13 @@
         <v>0.1</v>
       </c>
       <c r="J2">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="K2">
         <v>67</v>
       </c>
       <c r="L2">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="M2">
         <v>0</v>
@@ -1200,7 +1205,7 @@
         <v>75</v>
       </c>
       <c r="L3">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="M3">
         <v>0</v>
@@ -1235,13 +1240,13 @@
         <v>0.1</v>
       </c>
       <c r="J4">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="K4">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="L4">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="M4">
         <v>0</v>
@@ -1279,10 +1284,10 @@
         <v>2</v>
       </c>
       <c r="K5">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="L5">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="M5">
         <v>0</v>
@@ -1323,7 +1328,7 @@
         <v>62</v>
       </c>
       <c r="L6">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="M6">
         <v>0</v>
@@ -1364,7 +1369,7 @@
         <v>55</v>
       </c>
       <c r="L7">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="M7">
         <v>0</v>
@@ -1402,10 +1407,10 @@
         <v>3</v>
       </c>
       <c r="K8">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="L8">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="M8">
         <v>0</v>
@@ -1443,10 +1448,10 @@
         <v>5</v>
       </c>
       <c r="K9">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="L9">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="M9">
         <v>0</v>
@@ -1484,10 +1489,10 @@
         <v>2</v>
       </c>
       <c r="K10">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="L10">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="M10">
         <v>0</v>
@@ -1525,10 +1530,10 @@
         <v>2</v>
       </c>
       <c r="K11">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="L11">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="M11">
         <v>0</v>
@@ -1604,10 +1609,10 @@
         <v>0.1</v>
       </c>
       <c r="J13">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="K13">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="L13">
         <v>37</v>
@@ -1648,10 +1653,10 @@
         <v>2</v>
       </c>
       <c r="K14">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="L14">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="M14">
         <v>0</v>
@@ -1771,10 +1776,10 @@
         <v>2</v>
       </c>
       <c r="K17">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="L17">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="M17">
         <v>388000</v>
@@ -1856,7 +1861,7 @@
         <v>38</v>
       </c>
       <c r="L19">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="M19">
         <v>594000</v>
@@ -2102,7 +2107,7 @@
         <v>43</v>
       </c>
       <c r="L25">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="M25">
         <v>0</v>
@@ -2184,7 +2189,7 @@
         <v>78</v>
       </c>
       <c r="L27">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="M27">
         <v>2743374</v>
@@ -2342,10 +2347,10 @@
         <v>0.1</v>
       </c>
       <c r="J31">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="K31">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="L31">
         <v>59</v>
@@ -2386,10 +2391,10 @@
         <v>6</v>
       </c>
       <c r="K32">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="L32">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M32">
         <v>0</v>
@@ -2424,13 +2429,13 @@
         <v>0.1</v>
       </c>
       <c r="J33">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="K33">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="L33">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="M33">
         <v>0</v>
@@ -2465,7 +2470,7 @@
         <v>0.1</v>
       </c>
       <c r="J34">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="K34">
         <v>82</v>
@@ -2755,10 +2760,10 @@
         <v>4</v>
       </c>
       <c r="K41">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="L41">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="M41">
         <v>0</v>
@@ -2796,7 +2801,7 @@
         <v>4</v>
       </c>
       <c r="K42">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="L42">
         <v>37</v>
@@ -2809,10 +2814,10 @@
       <c r="A43">
         <v>2017</v>
       </c>
-      <c r="B43" s="3">
+      <c r="B43">
         <v>88197</v>
       </c>
-      <c r="C43" s="3">
+      <c r="C43">
         <v>0.05</v>
       </c>
       <c r="D43" t="s">
@@ -2833,33 +2838,33 @@
       <c r="I43">
         <v>0.1</v>
       </c>
-      <c r="J43" s="1">
+      <c r="J43">
         <v>3</v>
       </c>
-      <c r="K43" s="1">
+      <c r="K43">
         <v>68</v>
       </c>
-      <c r="L43" s="1">
+      <c r="L43">
         <v>29</v>
       </c>
       <c r="M43">
         <v>0</v>
       </c>
-      <c r="O43" s="2"/>
-      <c r="P43" s="2"/>
-      <c r="Q43" s="2"/>
-      <c r="S43" s="2"/>
-      <c r="T43" s="2"/>
-      <c r="U43" s="2"/>
+      <c r="O43" s="1"/>
+      <c r="P43" s="1"/>
+      <c r="Q43" s="1"/>
+      <c r="S43" s="1"/>
+      <c r="T43" s="1"/>
+      <c r="U43" s="1"/>
     </row>
     <row r="44" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>2018</v>
       </c>
-      <c r="B44" s="3">
+      <c r="B44">
         <v>108047</v>
       </c>
-      <c r="C44" s="3">
+      <c r="C44">
         <v>0.05</v>
       </c>
       <c r="D44" t="s">
@@ -2880,33 +2885,33 @@
       <c r="I44">
         <v>0.1</v>
       </c>
-      <c r="J44" s="1">
+      <c r="J44">
         <v>6</v>
       </c>
-      <c r="K44" s="1">
+      <c r="K44">
         <v>71</v>
       </c>
-      <c r="L44" s="1">
+      <c r="L44">
         <v>23</v>
       </c>
       <c r="M44">
         <v>0</v>
       </c>
-      <c r="O44" s="2"/>
-      <c r="P44" s="2"/>
-      <c r="Q44" s="2"/>
-      <c r="S44" s="2"/>
-      <c r="T44" s="2"/>
-      <c r="U44" s="2"/>
+      <c r="O44" s="1"/>
+      <c r="P44" s="1"/>
+      <c r="Q44" s="1"/>
+      <c r="S44" s="1"/>
+      <c r="T44" s="1"/>
+      <c r="U44" s="1"/>
     </row>
     <row r="45" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>2019</v>
       </c>
-      <c r="B45" s="3">
+      <c r="B45">
         <v>136090.58264235157</v>
       </c>
-      <c r="C45" s="3">
+      <c r="C45">
         <v>0.1</v>
       </c>
       <c r="D45" t="s">
@@ -2927,33 +2932,33 @@
       <c r="I45">
         <v>0.1</v>
       </c>
-      <c r="J45" s="1">
+      <c r="J45">
         <v>2</v>
       </c>
-      <c r="K45" s="1">
+      <c r="K45">
         <v>80</v>
       </c>
-      <c r="L45" s="1">
+      <c r="L45">
         <v>18</v>
       </c>
       <c r="M45">
         <v>0</v>
       </c>
-      <c r="O45" s="2"/>
-      <c r="P45" s="2"/>
-      <c r="Q45" s="2"/>
-      <c r="S45" s="2"/>
-      <c r="T45" s="2"/>
-      <c r="U45" s="2"/>
+      <c r="O45" s="1"/>
+      <c r="P45" s="1"/>
+      <c r="Q45" s="1"/>
+      <c r="S45" s="1"/>
+      <c r="T45" s="1"/>
+      <c r="U45" s="1"/>
     </row>
     <row r="46" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>2020</v>
       </c>
-      <c r="B46" s="3">
+      <c r="B46">
         <v>50745.526315789473</v>
       </c>
-      <c r="C46" s="3">
+      <c r="C46">
         <v>0.05</v>
       </c>
       <c r="D46" t="s">
@@ -2974,33 +2979,33 @@
       <c r="I46">
         <v>0.1</v>
       </c>
-      <c r="J46" s="1">
+      <c r="J46">
         <v>8</v>
       </c>
-      <c r="K46" s="1">
+      <c r="K46">
         <v>61</v>
       </c>
-      <c r="L46" s="1">
+      <c r="L46">
         <v>31</v>
       </c>
       <c r="M46">
         <v>0</v>
       </c>
-      <c r="O46" s="2"/>
-      <c r="P46" s="2"/>
-      <c r="Q46" s="2"/>
-      <c r="S46" s="2"/>
-      <c r="T46" s="2"/>
-      <c r="U46" s="2"/>
+      <c r="O46" s="1"/>
+      <c r="P46" s="1"/>
+      <c r="Q46" s="1"/>
+      <c r="S46" s="1"/>
+      <c r="T46" s="1"/>
+      <c r="U46" s="1"/>
     </row>
     <row r="47" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>2021</v>
       </c>
-      <c r="B47" s="3">
+      <c r="B47">
         <v>65199</v>
       </c>
-      <c r="C47" s="3">
+      <c r="C47">
         <v>0.05</v>
       </c>
       <c r="D47" t="s">
@@ -3021,33 +3026,33 @@
       <c r="I47">
         <v>0.1</v>
       </c>
-      <c r="J47" s="1">
+      <c r="J47">
         <v>27</v>
       </c>
-      <c r="K47" s="1">
+      <c r="K47">
         <v>58</v>
       </c>
-      <c r="L47" s="1">
+      <c r="L47">
         <v>16</v>
       </c>
       <c r="M47">
         <v>0</v>
       </c>
-      <c r="O47" s="2"/>
-      <c r="P47" s="2"/>
-      <c r="Q47" s="2"/>
-      <c r="S47" s="2"/>
-      <c r="T47" s="2"/>
-      <c r="U47" s="2"/>
+      <c r="O47" s="1"/>
+      <c r="P47" s="1"/>
+      <c r="Q47" s="1"/>
+      <c r="S47" s="1"/>
+      <c r="T47" s="1"/>
+      <c r="U47" s="1"/>
     </row>
     <row r="48" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>2022</v>
       </c>
-      <c r="B48" s="3">
+      <c r="B48">
         <v>100633.69019304212</v>
       </c>
-      <c r="C48" s="3">
+      <c r="C48">
         <v>0.1</v>
       </c>
       <c r="D48" t="s">
@@ -3068,24 +3073,24 @@
       <c r="I48">
         <v>0.1</v>
       </c>
-      <c r="J48" s="1">
-        <v>13</v>
-      </c>
-      <c r="K48" s="1">
+      <c r="J48">
+        <v>13</v>
+      </c>
+      <c r="K48">
         <v>75</v>
       </c>
-      <c r="L48" s="1">
-        <v>11</v>
+      <c r="L48">
+        <v>12</v>
       </c>
       <c r="M48">
         <v>0</v>
       </c>
-      <c r="O48" s="2"/>
-      <c r="P48" s="2"/>
-      <c r="Q48" s="2"/>
-      <c r="S48" s="2"/>
-      <c r="T48" s="2"/>
-      <c r="U48" s="2"/>
+      <c r="O48" s="1"/>
+      <c r="P48" s="1"/>
+      <c r="Q48" s="1"/>
+      <c r="S48" s="1"/>
+      <c r="T48" s="1"/>
+      <c r="U48" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
update csv coda output
</commit_message>
<xml_diff>
--- a/2023_analysis/data/chilkat_sockeye_template.xlsx
+++ b/2023_analysis/data/chilkat_sockeye_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Chilkat_sockeye_state_space_model\2023_analysis\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A129462D-5D61-4CBB-9677-875BB3C86F8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B7C35BF-5194-4488-A376-59EDF636B2B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="36915" yWindow="3870" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="chilkat_sockeye" sheetId="1" r:id="rId1"/>
@@ -38,6 +38,30 @@
     <author>NA</author>
   </authors>
   <commentList>
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{CFC9202C-8824-40EF-AF65-EB8C98F89A49}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Copy this sheet to the csv file that is needed for the model</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="B1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
@@ -57,7 +81,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">Make sure the spreadsheet Chilkat Lake DIDSON-daily counts 2008-2022 is updated to reflect any DIDSON expansion. This will carry over to the 'Chikat sockeye weighted age comp.' spreadsheet and the brood table spreadsheet, 'age' sheet. 
+          <t xml:space="preserve">Make sure the spreadsheet Chilkat Lake DIDSON-daily counts 2008-2022 is updated to reflect any DIDSON expansion. This will carry over to the 'Chikat sockeye weighted age comp.' spreadsheet and the brood table spreadsheet, 'age' sheet. ; S:\Region1Shared-DCF\Research\Salmon\Sockeye\Haines\Escapement Data\Chilkat Lake Weir\Chilkat Expanded Weir Counts
 </t>
         </r>
       </text>
@@ -81,7 +105,31 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">verify 0.05 if not expanded; 0.1 if expanded early OR late; 0.2 if expanded for both early and late
+          <t xml:space="preserve">0.05 if not expanded; 0.1 if expanded early OR late; 0.2 if expanded for both early and late
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{415330DA-C56F-42CC-88AA-8B49235AA424}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>S:\Region1Shared-DCF\Research\Salmon\Sockeye\Haines\Escapement Data\Chilkat Lake Weir\Chilkat Expanded Weir Counts; Chilkat Lake weir-daily counts 1971-2007.xlsx</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
 </t>
         </r>
       </text>
@@ -1083,7 +1131,7 @@
   <dimension ref="A1:U48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L22" sqref="L22"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>